<commit_message>
add dept1703, dept1704. adding more documentation
</commit_message>
<xml_diff>
--- a/UAL/output/dept1705/Daniel Martin_2022.xlsx
+++ b/UAL/output/dept1705/Daniel Martin_2022.xlsx
@@ -621,42 +621,42 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Daniel M. Martin, F Bäcker, B Deusinger, C Kubik, P Gehringer, J Schröder, Peter Groche</t>
+          <t>Daniel de Luis, O Izaola, D Primo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Technical University of Darmstadt, Institute for Production Engineering and Forming Machines Darmstadt, Germany; VACUUMSCHMELZE GmbH &amp; Co. KG, Hanau, Germany; Technical University of Darmstadt, Institute of Electrical Energy Conversion Darmstadt, Germany; Technical University of Darmstadt, Institute for Production Engineering and Forming Machines Darmstadt, Germany; Technical University of Darmstadt, Institute for Production Engineering and Forming Machines Darmstadt, Germany; VACUUMSCHMELZE GmbH &amp; Co. KG, Hanau, Germany; Technical University of Darmstadt, Institute for Production Engineering and Forming Machines Darmstadt, Germany</t>
+          <t xml:space="preserve">Department of Endocrinology and Nutrition, School of Medicine, Endocrinology and Nutrition Research Center, Hospital Clinico Universitario, University of Valladolid, Valladolid, Spain. dadluis@yahoo.es.; ; </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4281908789</t>
+          <t>https://openalex.org/W4306913082</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Design Guidelines for interlocked stator cores made of CoFe sheets</t>
+          <t>Effect of the variant rs602662 of FUT2 gene on anthropometric and metabolic parameters in a Caucasian obese population.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2022-05-01</t>
+          <t>2022-10-01</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>IOP Conference Series: Materials Science and Engineering</t>
+          <t>DOAJ (DOAJ: Directory of Open Access Journals)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>IOP Publishing</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1088/1757-899x/1238/1/012036</t>
+          <t>https://doaj.org/article/a05c41a7544544bda272b243672380e4</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -666,12 +666,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>publishedVersion</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>gold</t>
+          <t>closed</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -691,12 +691,12 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/36263525</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1088/1757-899x/1238/1/012036</t>
+          <t>https://doi.org/10.26355/eurrev_202210_29904</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -708,27 +708,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Daniel de Luis, O Izaola, D Primo</t>
+          <t>David Pacheco, Olatz Izaola, David Primo, Daniel de Luis</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Department of Endocrinology and Nutrition, School of Medicine, Endocrinology and Nutrition Research Center, Hospital Clinico Universitario, University of Valladolid, Valladolid, Spain. dadluis@yahoo.es.; ; </t>
+          <t xml:space="preserve">Center of Investigation of Endocrinology and Nutrition, School of Medicine, Department of Endocrinology and Nutrition, Hospital Clinico Universitario, University of Valladolid, Valladolid, Spain. dadluis@yahoo.es.; ; ; </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4306913082</t>
+          <t>https://openalex.org/W4205170538</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Effect of the variant rs602662 of FUT2 gene on anthropometric and metabolic parameters in a Caucasian obese population.</t>
+          <t>Role of the variant rs3774261 of adiponectin gene on adiponectin levels and ratio adiponectin/leptin after biliopancreatic diversion in morbid obese subjects.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2022-10-01</t>
+          <t>2022-01-01</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://doaj.org/article/a05c41a7544544bda272b243672380e4</t>
+          <t>https://doaj.org/article/749ba674ecf44978a913cbc170fa65a5</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -778,12 +778,12 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/36263525</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/35049001</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>https://doi.org/10.26355/eurrev_202210_29904</t>
+          <t>https://doi.org/10.26355/eurrev_202201_27774</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -795,42 +795,42 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>David Pacheco, Olatz Izaola, David Primo, Daniel de Luis</t>
+          <t>Daniel M. Martin, F Bäcker, B Deusinger, C Kubik, P Gehringer, J Schröder, Peter Groche</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Center of Investigation of Endocrinology and Nutrition, School of Medicine, Department of Endocrinology and Nutrition, Hospital Clinico Universitario, University of Valladolid, Valladolid, Spain. dadluis@yahoo.es.; ; ; </t>
+          <t>Technical University of Darmstadt, Institute for Production Engineering and Forming Machines Darmstadt, Germany; VACUUMSCHMELZE GmbH &amp; Co. KG, Hanau, Germany; Technical University of Darmstadt, Institute of Electrical Energy Conversion Darmstadt, Germany; Technical University of Darmstadt, Institute for Production Engineering and Forming Machines Darmstadt, Germany; Technical University of Darmstadt, Institute for Production Engineering and Forming Machines Darmstadt, Germany; VACUUMSCHMELZE GmbH &amp; Co. KG, Hanau, Germany; Technical University of Darmstadt, Institute for Production Engineering and Forming Machines Darmstadt, Germany</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4205170538</t>
+          <t>https://openalex.org/W4281908789</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Role of the variant rs3774261 of adiponectin gene on adiponectin levels and ratio adiponectin/leptin after biliopancreatic diversion in morbid obese subjects.</t>
+          <t>Design Guidelines for interlocked stator cores made of CoFe sheets</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-01-01</t>
+          <t>2022-05-01</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DOAJ (DOAJ: Directory of Open Access Journals)</t>
+          <t>IOP Conference Series: Materials Science and Engineering</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>IOP Publishing</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://doaj.org/article/749ba674ecf44978a913cbc170fa65a5</t>
+          <t>https://doi.org/10.1088/1757-899x/1238/1/012036</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -840,12 +840,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>publishedVersion</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>closed</t>
+          <t>gold</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -865,12 +865,12 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/35049001</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>https://doi.org/10.26355/eurrev_202201_27774</t>
+          <t>https://doi.org/10.1088/1757-899x/1238/1/012036</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">

</xml_diff>